<commit_message>
Lösung Netzplan Übung 2
</commit_message>
<xml_diff>
--- a/FIAED Übungen/Netzplan_Übung2.xlsx
+++ b/FIAED Übungen/Netzplan_Übung2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captiva\git\QM_PM\FIAED Übungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA0352E-E9E4-4D14-857C-2CA0E24E9E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2F3BFF-7FC0-4FE4-9AEF-23C68AB45FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -279,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -339,11 +339,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -456,11 +605,246 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -949,7 +1333,7 @@
   <dimension ref="A1:AD45"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1426,132 +1810,226 @@
       <c r="AD12" s="10"/>
     </row>
     <row r="13" spans="1:30">
-      <c r="A13" s="31"/>
+      <c r="A13" s="31">
+        <v>0</v>
+      </c>
       <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
+      <c r="C13" s="33">
+        <v>6</v>
+      </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="F13" s="31">
+        <v>6</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33">
+        <v>13</v>
+      </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="K13" s="31">
+        <v>13</v>
+      </c>
+      <c r="L13" s="32"/>
+      <c r="M13" s="33">
+        <v>18</v>
+      </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
+      <c r="P13" s="31">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="33">
+        <v>21</v>
+      </c>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
+      <c r="U13" s="31">
+        <v>21</v>
+      </c>
+      <c r="V13" s="32"/>
+      <c r="W13" s="33">
+        <v>24</v>
+      </c>
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
-      <c r="Z13" s="10"/>
-      <c r="AA13" s="10"/>
-      <c r="AB13" s="10"/>
+      <c r="Z13" s="31">
+        <v>26</v>
+      </c>
+      <c r="AA13" s="32"/>
+      <c r="AB13" s="33">
+        <v>35</v>
+      </c>
       <c r="AC13" s="10"/>
       <c r="AD13" s="10"/>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:30" ht="13.5" thickBot="1">
       <c r="A14" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="34"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14" s="10"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
+      <c r="X14" s="40"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="34"/>
       <c r="AC14" s="10"/>
       <c r="AD14" s="10"/>
     </row>
-    <row r="15" spans="1:30">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="10"/>
+    <row r="15" spans="1:30" ht="13.5" thickBot="1">
+      <c r="A15" s="35">
+        <v>6</v>
+      </c>
+      <c r="B15" s="36">
+        <v>0</v>
+      </c>
+      <c r="C15" s="37">
+        <v>0</v>
+      </c>
+      <c r="D15" s="42"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="F15" s="35">
+        <v>7</v>
+      </c>
+      <c r="G15" s="36">
+        <v>2</v>
+      </c>
+      <c r="H15" s="37">
+        <v>0</v>
+      </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="K15" s="35">
+        <v>5</v>
+      </c>
+      <c r="L15" s="36">
+        <v>2</v>
+      </c>
+      <c r="M15" s="37">
+        <v>0</v>
+      </c>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
+      <c r="P15" s="35">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="36">
+        <v>2</v>
+      </c>
+      <c r="R15" s="37">
+        <v>0</v>
+      </c>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
+      <c r="U15" s="35">
+        <v>3</v>
+      </c>
+      <c r="V15" s="36">
+        <v>2</v>
+      </c>
+      <c r="W15" s="37">
+        <v>2</v>
+      </c>
       <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10"/>
-      <c r="AA15" s="10"/>
-      <c r="AB15" s="10"/>
+      <c r="Y15" s="49"/>
+      <c r="Z15" s="35">
+        <v>9</v>
+      </c>
+      <c r="AA15" s="36">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="37">
+        <v>0</v>
+      </c>
       <c r="AC15" s="10"/>
       <c r="AD15" s="10"/>
     </row>
     <row r="16" spans="1:30">
-      <c r="A16" s="38"/>
+      <c r="A16" s="38">
+        <v>0</v>
+      </c>
       <c r="B16" s="32"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="10"/>
+      <c r="C16" s="39">
+        <v>6</v>
+      </c>
+      <c r="D16" s="43"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="F16" s="38">
+        <v>8</v>
+      </c>
+      <c r="G16" s="32"/>
+      <c r="H16" s="39">
+        <v>15</v>
+      </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
+      <c r="K16" s="38">
+        <v>15</v>
+      </c>
+      <c r="L16" s="32"/>
+      <c r="M16" s="39">
+        <v>20</v>
+      </c>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
+      <c r="P16" s="38">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="39">
+        <v>23</v>
+      </c>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
+      <c r="U16" s="38">
+        <v>23</v>
+      </c>
+      <c r="V16" s="32"/>
+      <c r="W16" s="39">
+        <v>26</v>
+      </c>
+      <c r="X16" s="47"/>
       <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="10"/>
+      <c r="Z16" s="38">
+        <v>26</v>
+      </c>
+      <c r="AA16" s="32"/>
+      <c r="AB16" s="39">
+        <v>35</v>
+      </c>
       <c r="AC16" s="10"/>
       <c r="AD16" s="10"/>
     </row>
@@ -1559,6 +2037,7 @@
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
+      <c r="D17" s="44"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1577,7 +2056,7 @@
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
+      <c r="X17" s="47"/>
       <c r="Y17" s="10"/>
       <c r="Z17" s="10"/>
       <c r="AA17" s="10"/>
@@ -1589,6 +2068,7 @@
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
+      <c r="D18" s="44"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
@@ -1607,7 +2087,7 @@
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
+      <c r="X18" s="47"/>
       <c r="Y18" s="10"/>
       <c r="Z18" s="10"/>
       <c r="AA18" s="10"/>
@@ -1619,25 +2099,38 @@
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="D19" s="44"/>
+      <c r="F19" s="31">
+        <v>6</v>
+      </c>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33">
+        <v>10</v>
+      </c>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
+      <c r="K19" s="31">
+        <v>10</v>
+      </c>
+      <c r="L19" s="32"/>
+      <c r="M19" s="33">
+        <v>19</v>
+      </c>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
+      <c r="P19" s="31">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="33">
+        <v>26</v>
+      </c>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
+      <c r="X19" s="47"/>
       <c r="Y19" s="10"/>
       <c r="Z19" s="10"/>
       <c r="AA19" s="10"/>
@@ -1645,26 +2138,34 @@
       <c r="AC19" s="10"/>
       <c r="AD19" s="10"/>
     </row>
-    <row r="20" spans="1:30">
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
+    <row r="20" spans="1:30" ht="13.5" thickBot="1">
+      <c r="D20" s="44"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="46"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="46"/>
+      <c r="X20" s="48"/>
       <c r="Y20" s="10"/>
       <c r="Z20" s="10"/>
       <c r="AA20" s="10"/>
@@ -1673,19 +2174,37 @@
       <c r="AD20" s="10"/>
     </row>
     <row r="21" spans="1:30">
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="F21" s="35">
+        <v>4</v>
+      </c>
+      <c r="G21" s="36">
+        <v>0</v>
+      </c>
+      <c r="H21" s="37">
+        <v>0</v>
+      </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
+      <c r="K21" s="35">
+        <v>9</v>
+      </c>
+      <c r="L21" s="36">
+        <v>0</v>
+      </c>
+      <c r="M21" s="37">
+        <v>0</v>
+      </c>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
+      <c r="P21" s="35">
+        <v>7</v>
+      </c>
+      <c r="Q21" s="36">
+        <v>0</v>
+      </c>
+      <c r="R21" s="37">
+        <v>0</v>
+      </c>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
       <c r="U21" s="10"/>
@@ -1700,19 +2219,31 @@
       <c r="AD21" s="10"/>
     </row>
     <row r="22" spans="1:30">
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="F22" s="38">
+        <v>6</v>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="H22" s="39">
+        <v>10</v>
+      </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
+      <c r="K22" s="38">
+        <v>10</v>
+      </c>
+      <c r="L22" s="32"/>
+      <c r="M22" s="39">
+        <v>19</v>
+      </c>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
+      <c r="P22" s="38">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="39">
+        <v>26</v>
+      </c>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
@@ -1953,27 +2484,75 @@
       <c r="C45" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="20">
     <mergeCell ref="R35:AB35"/>
     <mergeCell ref="D36:H36"/>
     <mergeCell ref="A37:A45"/>
     <mergeCell ref="C37:C45"/>
+    <mergeCell ref="K14:M14"/>
     <mergeCell ref="D33:H33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="D34:H34"/>
     <mergeCell ref="D35:H35"/>
     <mergeCell ref="J35:P35"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="Z14:AB14"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="P20:R20"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A14:C14"/>
+    <mergeCell ref="F14:H14"/>
   </mergeCells>
   <conditionalFormatting sqref="B35">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L15">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q15">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q21">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V15">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA15">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1988,7 +2567,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:C13"/>
@@ -1999,7 +2578,7 @@
     <col min="1" max="64" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:18">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2017,7 +2596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:18">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -2039,7 +2618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:18">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -2057,7 +2636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:18">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2075,7 +2654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:18">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -2095,7 +2674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:18">
       <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
@@ -2111,27 +2690,217 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="31"/>
+    <row r="10" spans="1:18">
+      <c r="A10" s="31">
+        <v>0</v>
+      </c>
       <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="C10" s="33">
+        <f>A10+A12</f>
+        <v>6</v>
+      </c>
+      <c r="F10" s="31">
+        <f>C10</f>
+        <v>6</v>
+      </c>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33">
+        <f>F10+F12</f>
+        <v>13</v>
+      </c>
+      <c r="K10" s="31">
+        <f>MAX(H10,H16)</f>
+        <v>13</v>
+      </c>
+      <c r="L10" s="32"/>
+      <c r="M10" s="33">
+        <f>K10+K12</f>
+        <v>18</v>
+      </c>
+      <c r="P10" s="31">
+        <f>M10</f>
+        <v>18</v>
+      </c>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="33">
+        <f>P10+P12</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="13.5" thickBot="1">
       <c r="A11" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="35"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="38"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+    </row>
+    <row r="12" spans="1:18" ht="13.5" thickBot="1">
+      <c r="A12" s="35">
+        <f>VLOOKUP(A11,$A$2:$H$6,8)</f>
+        <v>6</v>
+      </c>
+      <c r="B12" s="36">
+        <f>C13-C10</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="37">
+        <f>MIN(F10,F16)-C10</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="52"/>
+      <c r="F12" s="35">
+        <f>VLOOKUP(F11,$A$2:$H$6,8)</f>
+        <v>7</v>
+      </c>
+      <c r="G12" s="36">
+        <f>H13-H10</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="37">
+        <f>K10-H10</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="35">
+        <f>VLOOKUP(K11,$A$2:$H$6,8)</f>
+        <v>5</v>
+      </c>
+      <c r="L12" s="36">
+        <f>M13-M10</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="37">
+        <f>P10-M10</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="35">
+        <f>VLOOKUP(P11,$A$2:$H$6,8)</f>
+        <v>9</v>
+      </c>
+      <c r="Q12" s="36">
+        <f>R13-R10</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="38">
+        <f>C13-A12</f>
+        <v>0</v>
+      </c>
       <c r="B13" s="32"/>
-      <c r="C13" s="39"/>
+      <c r="C13" s="39">
+        <f>MIN(F13,F19)</f>
+        <v>6</v>
+      </c>
+      <c r="D13" s="53"/>
+      <c r="F13" s="38">
+        <f>H13-F12</f>
+        <v>6</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="39">
+        <f>K13</f>
+        <v>13</v>
+      </c>
+      <c r="I13" s="44"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="38">
+        <f>M13-K12</f>
+        <v>13</v>
+      </c>
+      <c r="L13" s="32"/>
+      <c r="M13" s="39">
+        <f>P13</f>
+        <v>18</v>
+      </c>
+      <c r="P13" s="38">
+        <f>R13-P12</f>
+        <v>18</v>
+      </c>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="39">
+        <f>R10</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="D14" s="44"/>
+      <c r="I14" s="44"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="D15" s="44"/>
+      <c r="I15" s="44"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="D16" s="44"/>
+      <c r="F16" s="31">
+        <f>C10</f>
+        <v>6</v>
+      </c>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33">
+        <f>F16+F18</f>
+        <v>10</v>
+      </c>
+      <c r="I16" s="44"/>
+    </row>
+    <row r="17" spans="4:9" ht="13.5" thickBot="1">
+      <c r="D17" s="44"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="54"/>
+    </row>
+    <row r="18" spans="4:9">
+      <c r="F18" s="35">
+        <f>VLOOKUP(F17,$A$2:$H$6,8)</f>
+        <v>4</v>
+      </c>
+      <c r="G18" s="36">
+        <f>H19-H16</f>
+        <v>3</v>
+      </c>
+      <c r="H18" s="37">
+        <f>K10-H16</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9">
+      <c r="F19" s="38">
+        <f>H19-F18</f>
+        <v>9</v>
+      </c>
+      <c r="G19" s="32"/>
+      <c r="H19" s="39">
+        <f>K13</f>
+        <v>13</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="13.5">
       <c r="A40" s="24"/>
@@ -2376,7 +3145,7 @@
       <c r="L53" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
     <mergeCell ref="C47:K47"/>
     <mergeCell ref="C48:K48"/>
     <mergeCell ref="C49:K49"/>
@@ -2386,16 +3155,40 @@
     <mergeCell ref="F42:J42"/>
     <mergeCell ref="C46:K46"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="P11:R11"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C42:C43 B51">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q12">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2410,10 +3203,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63E01CD-865F-4E26-A853-50A2EF61E747}">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -2421,7 +3214,7 @@
     <col min="1" max="64" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:18">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2439,7 +3232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:18">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -2463,7 +3256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:18">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -2481,7 +3274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:18">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -2499,7 +3292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:18">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -2517,7 +3310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:18">
       <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
@@ -2535,7 +3328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:18">
       <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2553,7 +3346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:18">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -2573,27 +3366,327 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="31"/>
+    <row r="11" spans="1:18">
+      <c r="A11" s="31">
+        <v>0</v>
+      </c>
       <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="C11" s="33">
+        <f>A11+A13</f>
+        <v>2</v>
+      </c>
+      <c r="F11" s="31">
+        <f>C$11</f>
+        <v>2</v>
+      </c>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33">
+        <f>F11+F13</f>
+        <v>13</v>
+      </c>
+      <c r="P11" s="31">
+        <f>MAX(M17,M23)</f>
+        <v>17</v>
+      </c>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="33">
+        <f>P11+P13</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="13.5" thickBot="1">
       <c r="A12" s="34" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="35"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="38"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+    </row>
+    <row r="13" spans="1:18" ht="13.5" thickBot="1">
+      <c r="A13" s="35">
+        <f>VLOOKUP(A12,$A$2:$H$8,8)</f>
+        <v>2</v>
+      </c>
+      <c r="B13" s="36">
+        <f>C14-C11</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="37">
+        <f>MIN(F11,F17,F23)-C11</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="52"/>
+      <c r="F13" s="35">
+        <f>VLOOKUP(F12,$A$2:$H$6,8)</f>
+        <v>11</v>
+      </c>
+      <c r="G13" s="36">
+        <f>H14-H11</f>
+        <v>4</v>
+      </c>
+      <c r="H13" s="37">
+        <f>P11-H11</f>
+        <v>4</v>
+      </c>
+      <c r="O13" s="59"/>
+      <c r="P13" s="35">
+        <f>VLOOKUP(P12,$A$2:$H$8,8)</f>
+        <v>9</v>
+      </c>
+      <c r="Q13" s="36">
+        <f>R14-R11</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="37"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="38">
+        <f>C14-A13</f>
+        <v>0</v>
+      </c>
       <c r="B14" s="32"/>
-      <c r="C14" s="39"/>
+      <c r="C14" s="39">
+        <f>MIN(F11,F17,F23)</f>
+        <v>2</v>
+      </c>
+      <c r="D14" s="53"/>
+      <c r="F14" s="38">
+        <f>H14-F13</f>
+        <v>6</v>
+      </c>
+      <c r="G14" s="32"/>
+      <c r="H14" s="39">
+        <f>P14</f>
+        <v>17</v>
+      </c>
+      <c r="N14" s="44"/>
+      <c r="P14" s="38">
+        <f>R14-P13</f>
+        <v>17</v>
+      </c>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="39">
+        <f>R11</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="C15" s="56"/>
+      <c r="D15" s="44"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+    </row>
+    <row r="17" spans="3:15">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="F17" s="31">
+        <f>C$11</f>
+        <v>2</v>
+      </c>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33">
+        <f>F17+F19</f>
+        <v>6</v>
+      </c>
+      <c r="K17" s="31">
+        <f>H17</f>
+        <v>6</v>
+      </c>
+      <c r="L17" s="32"/>
+      <c r="M17" s="33">
+        <f>K17+K19</f>
+        <v>9</v>
+      </c>
+      <c r="N17" s="44"/>
+      <c r="O17" s="44"/>
+    </row>
+    <row r="18" spans="3:15" ht="13.5" thickBot="1">
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="44"/>
+    </row>
+    <row r="19" spans="3:15">
+      <c r="C19" s="44"/>
+      <c r="F19" s="35">
+        <f>VLOOKUP(F18,$A$2:$H$6,8)</f>
+        <v>4</v>
+      </c>
+      <c r="G19" s="36">
+        <f>H20-H17</f>
+        <v>8</v>
+      </c>
+      <c r="H19" s="37">
+        <f>K17-H17</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="35">
+        <f>VLOOKUP(K18,$A$2:$H$6,8)</f>
+        <v>3</v>
+      </c>
+      <c r="L19" s="36">
+        <f>M20-M17</f>
+        <v>8</v>
+      </c>
+      <c r="M19" s="37">
+        <f>P$11-M17</f>
+        <v>8</v>
+      </c>
+      <c r="O19" s="44"/>
+    </row>
+    <row r="20" spans="3:15">
+      <c r="C20" s="44"/>
+      <c r="F20" s="38">
+        <f>H20-F19</f>
+        <v>10</v>
+      </c>
+      <c r="G20" s="32"/>
+      <c r="H20" s="39">
+        <f>K20</f>
+        <v>14</v>
+      </c>
+      <c r="K20" s="38">
+        <f>M20-K19</f>
+        <v>14</v>
+      </c>
+      <c r="L20" s="32"/>
+      <c r="M20" s="39">
+        <f>P$14</f>
+        <v>17</v>
+      </c>
+      <c r="O20" s="44"/>
+    </row>
+    <row r="21" spans="3:15">
+      <c r="C21" s="44"/>
+      <c r="O21" s="44"/>
+    </row>
+    <row r="22" spans="3:15">
+      <c r="C22" s="44"/>
+      <c r="O22" s="44"/>
+    </row>
+    <row r="23" spans="3:15">
+      <c r="C23" s="44"/>
+      <c r="F23" s="31">
+        <f>C$11</f>
+        <v>2</v>
+      </c>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33">
+        <f>F23+F25</f>
+        <v>10</v>
+      </c>
+      <c r="K23" s="31">
+        <f>H23</f>
+        <v>10</v>
+      </c>
+      <c r="L23" s="32"/>
+      <c r="M23" s="33">
+        <f>K23+K25</f>
+        <v>17</v>
+      </c>
+      <c r="O23" s="44"/>
+    </row>
+    <row r="24" spans="3:15" ht="13.5" thickBot="1">
+      <c r="C24" s="44"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="60"/>
+    </row>
+    <row r="25" spans="3:15">
+      <c r="F25" s="35">
+        <f>VLOOKUP(F24,$A$2:$H$6,8)</f>
+        <v>8</v>
+      </c>
+      <c r="G25" s="36">
+        <f>H26-H23</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="37">
+        <f>K23-H23</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="35">
+        <f>VLOOKUP(K24,$A$2:$H$8,8)</f>
+        <v>7</v>
+      </c>
+      <c r="L25" s="36">
+        <f>M26-M23</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="37">
+        <f>P$11-M23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15">
+      <c r="F26" s="38">
+        <f>H26-F25</f>
+        <v>2</v>
+      </c>
+      <c r="G26" s="32"/>
+      <c r="H26" s="39">
+        <f>K26</f>
+        <v>10</v>
+      </c>
+      <c r="K26" s="38">
+        <f>M26-K25</f>
+        <v>10</v>
+      </c>
+      <c r="L26" s="32"/>
+      <c r="M26" s="39">
+        <f>P$14</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="13.5">
       <c r="A42" s="24"/>
@@ -2838,12 +3931,18 @@
       <c r="L55" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="17">
+    <mergeCell ref="P12:R12"/>
     <mergeCell ref="C50:K50"/>
     <mergeCell ref="C51:K51"/>
     <mergeCell ref="C52:K52"/>
     <mergeCell ref="C53:K53"/>
     <mergeCell ref="A12:C12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K24:M24"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="B44:D44"/>
@@ -2852,7 +3951,37 @@
     <mergeCell ref="C49:K49"/>
   </mergeCells>
   <conditionalFormatting sqref="C44:C45 B53">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L25">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q13">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>